<commit_message>
added new rows during testing
</commit_message>
<xml_diff>
--- a/Evidencia_nezhod.xlsx
+++ b/Evidencia_nezhod.xlsx
@@ -1,99 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
-  <si>
-    <t>číslo objednávky</t>
-  </si>
-  <si>
-    <t>dopravca</t>
-  </si>
-  <si>
-    <t>dátum</t>
-  </si>
-  <si>
-    <t>komentár</t>
-  </si>
-  <si>
-    <t>dispečer CEVA Logistic</t>
-  </si>
-  <si>
-    <t>typ nezhody</t>
-  </si>
-  <si>
-    <t>koreňová príčina</t>
-  </si>
-  <si>
-    <t>T0000000000</t>
-  </si>
-  <si>
-    <t>testovanie84@gmail.com</t>
-  </si>
-  <si>
-    <t>2024-01-21</t>
-  </si>
-  <si>
-    <t>Nákladka je vykonaná.</t>
-  </si>
-  <si>
-    <t>Vozidlo bude meškať na nákladku z dôvodu Dopravná nehoda. Predpokladaný čas nákladky: 2024-01-21 15:27</t>
-  </si>
-  <si>
-    <t>Vozidlo bude meškať na výkladku z dôvodu Iný dôvod. Predpokladaný čas výkladky: 2024-01-21 15:28</t>
-  </si>
-  <si>
-    <t>Admin</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>hopa</t>
-  </si>
-  <si>
-    <t>Dopravná nehoda</t>
-  </si>
-  <si>
-    <t>Iný dôvod</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -108,35 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -424,100 +420,321 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>číslo objednávky</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>dopravca</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>dátum</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>komentár</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>dispečer CEVA Logistic</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>typ nezhody</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>koreňová príčina</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>T0000000000</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>testovanie84@gmail.com</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>2024-01-21</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Nákladka je vykonaná.</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>T0000000000</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>testovanie84@gmail.com</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2024-01-21</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Vozidlo bude meškať na nákladku z dôvodu Dopravná nehoda. Predpokladaný čas nákladky: 2024-01-21 15:27</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Dopravná nehoda</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>T0000000000</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>testovanie84@gmail.com</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2024-01-21</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Vozidlo bude meškať na výkladku z dôvodu Iný dôvod. Predpokladaný čas výkladky: 2024-01-21 15:28</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>hopa</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Iný dôvod</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>T0000000000</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>testovanie84@gmail.com</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2024-01-21</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Výkladka je vykonaná.</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>T0000000000</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>testovanie84@gmail.com</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2024-01-21</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Vozidlo bude meškať na nákladku z dôvodu Nepriaznivé počasie. Predpokladaný čas nákladky: 2024-01-22 10:00</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Nepriaznivé počasie</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>T0000000000</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>testovanie84@gmail.com</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2024-01-21</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Vozidlo bude meškať na výkladku z dôvodu Nepriaznivé počasie. Predpokladaný čas výkladky: 2024-01-21 22:02</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Nepriaznivé počasie</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>T0000000000</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>testovanie84@gmail.com</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2024-01-21</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Nákladka je vykonaná.</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr"/>
+      <c r="G8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>T0000000000</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>testovanie84@gmail.com</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2024-01-21</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Nákladka je vykonaná.</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Admin</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
zobrazenie stranky po odpovedi (#46)
</commit_message>
<xml_diff>
--- a/Evidencia_nezhod.xlsx
+++ b/Evidencia_nezhod.xlsx
@@ -1,37 +1,102 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarag\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4692B60-4076-4ECF-8BE6-8AF64896663F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="18">
+  <si>
+    <t>INES carrier file</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Responsible´s name</t>
+  </si>
+  <si>
+    <t>Type of non-conformity</t>
+  </si>
+  <si>
+    <t>Root cause</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Recorded by</t>
+  </si>
+  <si>
+    <t>T0000000000</t>
+  </si>
+  <si>
+    <t>2024-01-22</t>
+  </si>
+  <si>
+    <t>testovanie</t>
+  </si>
+  <si>
+    <t>Nakládka</t>
+  </si>
+  <si>
+    <t>Pokazený kamión</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Vykládka</t>
+  </si>
+  <si>
+    <t>Iný dôvod</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Dopravná nehoda</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +111,43 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,165 +435,105 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="25.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>INES carrier file</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Date</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Responsible´s name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Type of non-conformity</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Root cause</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Comment</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Recorded by</t>
-        </is>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>T0000000000</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2024-01-22</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>testovanie</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Nakládka</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Pokazený kamión</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>T0000000000</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>2024-01-22</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>testovanie</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Vykládka</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Iný dôvod</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Test</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>T0000000000</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2024-01-22</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>testovanie</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Nakládka</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Dopravná nehoda</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Admin</t>
-        </is>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
automatické sťahovanie príloh (#52)
</commit_message>
<xml_diff>
--- a/Evidencia_nezhod.xlsx
+++ b/Evidencia_nezhod.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarag\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarag\Desktop\kontrola-dorucenia-Sara\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A693C227-D63E-41AC-9A51-286FBD8F0D9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A081E7CF-05D7-4E03-A095-B14AD87A9041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30" yWindow="30" windowWidth="23970" windowHeight="12870" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>INES carrier file</t>
   </si>
@@ -59,63 +59,6 @@
   </si>
   <si>
     <t>Recorded by</t>
-  </si>
-  <si>
-    <t>T0000000000</t>
-  </si>
-  <si>
-    <t>2024-02-08</t>
-  </si>
-  <si>
-    <t>testovanie</t>
-  </si>
-  <si>
-    <t>2023-08-02</t>
-  </si>
-  <si>
-    <t>04:30:00</t>
-  </si>
-  <si>
-    <t>18:00:00</t>
-  </si>
-  <si>
-    <t>2024-02-28</t>
-  </si>
-  <si>
-    <t>14:47</t>
-  </si>
-  <si>
-    <t>14:51</t>
-  </si>
-  <si>
-    <t>20:02</t>
-  </si>
-  <si>
-    <t>Nakládka</t>
-  </si>
-  <si>
-    <t>Vykládka</t>
-  </si>
-  <si>
-    <t>Pokazený kamión</t>
-  </si>
-  <si>
-    <t>Iný dôvod</t>
-  </si>
-  <si>
-    <t>Zdržanie na predchádzajúcej výkladke</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>Komentár</t>
-  </si>
-  <si>
-    <t>Dôvod meškania</t>
-  </si>
-  <si>
-    <t>Tester User</t>
   </si>
 </sst>
 </file>
@@ -483,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +443,7 @@
     <col min="9" max="9" width="8.7109375" customWidth="1"/>
     <col min="10" max="10" width="22.7109375" customWidth="1"/>
     <col min="11" max="11" width="36.7109375" customWidth="1"/>
-    <col min="12" max="12" width="14.7109375" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" customWidth="1"/>
     <col min="13" max="13" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -545,129 +488,6 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L2" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M4" t="s">
-        <v>31</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>